<commit_message>
added e2e test, smoke changed
</commit_message>
<xml_diff>
--- a/Smoke чеклист для прооверки приложения ToDo List.xlsx
+++ b/Smoke чеклист для прооверки приложения ToDo List.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="51">
   <si>
     <t>Приложение</t>
   </si>
@@ -153,6 +153,9 @@
     <t>Все листы успешно удаляются</t>
   </si>
   <si>
+    <t>Использование в ландшафтном режиме</t>
+  </si>
+  <si>
     <t>Сортировка методом "By done" при отсутсвии листов задач</t>
   </si>
   <si>
@@ -169,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -177,10 +180,6 @@
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -222,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -239,7 +238,7 @@
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -248,16 +247,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5578,7 +5571,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="3"/>
@@ -5602,10 +5595,10 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -5613,10 +5606,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -5624,10 +5617,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -5635,29 +5628,29 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
@@ -10603,7 +10596,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4.0" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B6" sqref="B6" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
@@ -10624,7 +10620,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3"/>
@@ -10802,10 +10798,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -10813,10 +10809,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -10824,31 +10820,37 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="B22" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>47</v>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="s">
+        <v>50</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="8"/>
@@ -15715,24 +15717,29 @@
       <c r="B996" s="8"/>
       <c r="C996" s="3"/>
     </row>
+    <row r="997">
+      <c r="A997" s="8"/>
+      <c r="B997" s="8"/>
+      <c r="C997" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C996">
+  <conditionalFormatting sqref="C1:C997">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C996">
+  <conditionalFormatting sqref="C1:C997">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C996">
+  <conditionalFormatting sqref="C1:C997">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C996">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C997">
       <formula1>"OK,FAIL,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>